<commit_message>
Final changes to handle retry
</commit_message>
<xml_diff>
--- a/files/TARRANT COUNTY.xlsx
+++ b/files/TARRANT COUNTY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valeriezennmagbanua/Projects/Personal/Tool/address-scrape-tool/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA444DF-A630-994F-809D-3683DC3A6117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BE738B-03F2-8A45-8868-203E4003284C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="18000" windowHeight="20920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="M-Apr11" sheetId="1" r:id="rId1"/>
@@ -28561,7 +28561,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>